<commit_message>
3D and 2D Options
</commit_message>
<xml_diff>
--- a/setups/Var_Table_GCI_Pictures.xlsx
+++ b/setups/Var_Table_GCI_Pictures.xlsx
@@ -423,13 +423,13 @@
         <v>4</v>
       </c>
       <c r="C2">
-        <v>0.8733316393119919</v>
+        <v>0.4305099655428042</v>
       </c>
       <c r="D2">
-        <v>0.8702418810835432</v>
+        <v>0.4289701383089291</v>
       </c>
       <c r="E2">
-        <v>0.8706835263412515</v>
+        <v>0.4275098360405326</v>
       </c>
     </row>
     <row r="3" spans="1:5">
@@ -440,13 +440,13 @@
         <v>5</v>
       </c>
       <c r="C3">
-        <v>0.2329492598563525</v>
+        <v>0.08444725529611972</v>
       </c>
       <c r="D3">
-        <v>0.2376457028685719</v>
+        <v>0.08885734646265671</v>
       </c>
       <c r="E3">
-        <v>0.2377818330927085</v>
+        <v>0.08941429023735328</v>
       </c>
     </row>
     <row r="4" spans="1:5">
@@ -457,13 +457,13 @@
         <v>6</v>
       </c>
       <c r="C4">
-        <v>0.05426535766762242</v>
+        <v>0.007131338927048022</v>
       </c>
       <c r="D4">
-        <v>0.05647548009189757</v>
+        <v>0.007895628020384611</v>
       </c>
       <c r="E4">
-        <v>0.0565402001489287</v>
+        <v>0.00799491529864965</v>
       </c>
     </row>
     <row r="5" spans="1:5">
@@ -474,13 +474,13 @@
         <v>7</v>
       </c>
       <c r="C5">
-        <v>26.67363111221634</v>
+        <v>19.61563309914214</v>
       </c>
       <c r="D5">
-        <v>27.30800574349259</v>
+        <v>20.71411003407999</v>
       </c>
       <c r="E5">
-        <v>27.30978890710211</v>
+        <v>20.91514222584479</v>
       </c>
     </row>
   </sheetData>

</xml_diff>